<commit_message>
A few exploratory plots (e.g. Preferences by individual), exploration of how to compare the differences in preferences between the two sepcies.
</commit_message>
<xml_diff>
--- a/first_response_08.06.08.xlsx
+++ b/first_response_08.06.08.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maydixon/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maydixon/GitHub/Sensory_learning/Sensory_learning_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9C5A64-272C-8244-BB70-F37DBC87FAB9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248F1F08-EE69-A44F-B69B-41FCD41CD404}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6560" yWindow="460" windowWidth="24240" windowHeight="13160" xr2:uid="{DF475BE4-B537-9142-8DC1-1367596F23A7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="75">
   <si>
     <t>Bat ID</t>
   </si>
@@ -250,16 +250,13 @@
   </si>
   <si>
     <t>Rewarded_2</t>
-  </si>
-  <si>
-    <t>smll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -636,12 +633,12 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+      <selection sqref="A1:K82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -676,7 +673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -711,7 +708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -746,7 +743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -781,7 +778,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -816,7 +813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -851,7 +848,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -886,7 +883,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -921,7 +918,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -956,7 +953,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -991,7 +988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1026,7 +1023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1061,7 +1058,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1096,7 +1093,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1131,7 +1128,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1166,7 +1163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1201,7 +1198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1236,7 +1233,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -1271,7 +1268,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1306,7 +1303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -1341,7 +1338,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1376,7 +1373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1411,7 +1408,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1446,7 +1443,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -1481,7 +1478,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -1516,7 +1513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1551,7 +1548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1586,7 +1583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1621,7 +1618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1656,7 +1653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1691,7 +1688,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -1726,7 +1723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1761,7 +1758,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1796,7 +1793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1831,7 +1828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1866,7 +1863,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11">
       <c r="A36" s="3" t="s">
         <v>42</v>
       </c>
@@ -1901,7 +1898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1936,7 +1933,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -1971,7 +1968,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
@@ -2006,7 +2003,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -2041,7 +2038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2076,7 +2073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -2111,7 +2108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -2146,7 +2143,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2181,7 +2178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -2216,7 +2213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11">
       <c r="A46" s="3" t="s">
         <v>50</v>
       </c>
@@ -2251,7 +2248,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -2286,7 +2283,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -2321,7 +2318,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -2356,7 +2353,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2391,7 +2388,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -2426,7 +2423,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>23</v>
       </c>
@@ -2461,7 +2458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>27</v>
       </c>
@@ -2496,7 +2493,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="A54" s="6" t="s">
         <v>9</v>
       </c>
@@ -2531,7 +2528,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -2566,7 +2563,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>35</v>
       </c>
@@ -2601,7 +2598,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -2636,7 +2633,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>49</v>
       </c>
@@ -2671,7 +2668,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -2706,7 +2703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>42</v>
       </c>
@@ -2741,7 +2738,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>41</v>
       </c>
@@ -2773,7 +2770,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62" t="s">
         <v>16</v>
       </c>
@@ -2808,7 +2805,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>52</v>
       </c>
@@ -2843,123 +2840,123 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B64" s="9" t="s">
+    <row r="64" spans="1:11">
+      <c r="A64" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C64" s="10">
-        <v>43024</v>
-      </c>
-      <c r="D64" s="11">
-        <v>0.87430555555555556</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F64" s="9" t="s">
+      <c r="C64" s="4">
+        <v>42856</v>
+      </c>
+      <c r="D64" s="5">
+        <v>0.12430555555555556</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" t="s">
         <v>67</v>
       </c>
-      <c r="G64" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="H64" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="I64" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="J64" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="K64" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B65" s="3" t="s">
+      <c r="G64" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" t="s">
         <v>37</v>
       </c>
-      <c r="C65" s="4">
-        <v>42856</v>
-      </c>
-      <c r="D65" s="5">
-        <v>0.12430555555555556</v>
-      </c>
-      <c r="E65" s="3" t="s">
+      <c r="C65" s="1">
+        <v>42855</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E65" t="s">
         <v>11</v>
       </c>
       <c r="F65" t="s">
         <v>67</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="G65" t="s">
         <v>21</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H65" t="s">
         <v>58</v>
       </c>
-      <c r="I65" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I65" t="s">
+        <v>17</v>
+      </c>
+      <c r="J65" t="s">
+        <v>22</v>
+      </c>
+      <c r="K65" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
       <c r="A66" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C66" s="1">
-        <v>42855</v>
+        <v>43024</v>
       </c>
       <c r="D66" s="2">
-        <v>0.83333333333333337</v>
+        <v>0.87430555555555556</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F66" t="s">
         <v>67</v>
       </c>
       <c r="G66" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="H66" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="I66" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="J66" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="K66" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
       <c r="A67" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B67" t="s">
         <v>43</v>
       </c>
       <c r="C67" s="1">
-        <v>43024</v>
+        <v>43026</v>
       </c>
       <c r="D67" s="2">
-        <v>0.87430555555555556</v>
+        <v>0.79513888888888884</v>
       </c>
       <c r="E67" t="s">
         <v>25</v>
@@ -2974,97 +2971,97 @@
         <v>63</v>
       </c>
       <c r="I67" t="s">
+        <v>22</v>
+      </c>
+      <c r="J67" t="s">
+        <v>44</v>
+      </c>
+      <c r="K67" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D68" s="5">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I68" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="J67" t="s">
+      <c r="J68" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K68" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="K67" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>51</v>
-      </c>
-      <c r="B68" t="s">
-        <v>43</v>
-      </c>
-      <c r="C68" s="1">
-        <v>43026</v>
-      </c>
-      <c r="D68" s="2">
-        <v>0.79513888888888884</v>
-      </c>
-      <c r="E68" t="s">
-        <v>25</v>
-      </c>
-      <c r="F68" t="s">
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" s="1">
+        <v>42828</v>
+      </c>
+      <c r="D69" t="s">
+        <v>22</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
         <v>67</v>
       </c>
-      <c r="G68" t="s">
-        <v>48</v>
-      </c>
-      <c r="H68" t="s">
-        <v>63</v>
-      </c>
-      <c r="I68" t="s">
-        <v>22</v>
-      </c>
-      <c r="J68" t="s">
-        <v>44</v>
-      </c>
-      <c r="K68" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D69" s="5">
-        <v>8.8888888888888892E-2</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G69" s="3" t="s">
+      <c r="G69" t="s">
         <v>21</v>
       </c>
-      <c r="H69" s="3" t="s">
+      <c r="H69" t="s">
         <v>58</v>
       </c>
-      <c r="I69" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I69" t="s">
+        <v>17</v>
+      </c>
+      <c r="J69" t="s">
+        <v>22</v>
+      </c>
+      <c r="K69" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
       <c r="A70" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B70" t="s">
         <v>64</v>
       </c>
       <c r="C70" s="1">
-        <v>42828</v>
-      </c>
-      <c r="D70" t="s">
-        <v>22</v>
+        <v>42829</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.89930555555555547</v>
       </c>
       <c r="E70" t="s">
         <v>11</v>
@@ -3073,33 +3070,33 @@
         <v>67</v>
       </c>
       <c r="G70" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H70" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I70" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="J70" t="s">
         <v>22</v>
       </c>
       <c r="K70" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
       <c r="A71" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B71" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="C71" s="1">
-        <v>42829</v>
+        <v>42830</v>
       </c>
       <c r="D71" s="2">
-        <v>0.89930555555555547</v>
+        <v>0.92569444444444438</v>
       </c>
       <c r="E71" t="s">
         <v>11</v>
@@ -3123,18 +3120,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C72" s="1">
-        <v>42830</v>
+        <v>42856</v>
       </c>
       <c r="D72" s="2">
-        <v>0.92569444444444438</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="E72" t="s">
         <v>11</v>
@@ -3143,33 +3140,33 @@
         <v>67</v>
       </c>
       <c r="G72" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H72" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I72" t="s">
+        <v>44</v>
+      </c>
+      <c r="J72" t="s">
         <v>62</v>
       </c>
-      <c r="J72" t="s">
-        <v>22</v>
-      </c>
       <c r="K72" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B73" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C73" s="1">
-        <v>42856</v>
+        <v>42855</v>
       </c>
       <c r="D73" s="2">
-        <v>1.3888888888888888E-2</v>
+        <v>0.83888888888888891</v>
       </c>
       <c r="E73" t="s">
         <v>11</v>
@@ -3184,39 +3181,39 @@
         <v>58</v>
       </c>
       <c r="I73" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="J73" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K73" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B74" t="s">
         <v>66</v>
       </c>
       <c r="C74" s="1">
-        <v>42855</v>
+        <v>42945</v>
       </c>
       <c r="D74" s="2">
-        <v>0.83888888888888891</v>
+        <v>0.81527777777777777</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F74" t="s">
         <v>67</v>
       </c>
       <c r="G74" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I74" t="s">
         <v>55</v>
@@ -3228,9 +3225,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11">
       <c r="A75" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B75" t="s">
         <v>66</v>
@@ -3239,7 +3236,7 @@
         <v>42945</v>
       </c>
       <c r="D75" s="2">
-        <v>0.81527777777777777</v>
+        <v>0.87291666666666667</v>
       </c>
       <c r="E75" t="s">
         <v>25</v>
@@ -3263,30 +3260,30 @@
         <v>55</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11">
       <c r="A76" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B76" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="C76" s="1">
-        <v>42945</v>
+        <v>42855</v>
       </c>
       <c r="D76" s="2">
-        <v>0.87291666666666667</v>
+        <v>2.1527777777777781E-2</v>
       </c>
       <c r="E76" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F76" t="s">
         <v>67</v>
       </c>
       <c r="G76" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H76" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I76" t="s">
         <v>55</v>
@@ -3298,30 +3295,30 @@
         <v>55</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>49</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="77" spans="1:11">
+      <c r="A77" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B77" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C77" s="1">
-        <v>42855</v>
-      </c>
-      <c r="D77" s="2">
-        <v>2.1527777777777781E-2</v>
-      </c>
-      <c r="E77" t="s">
-        <v>11</v>
-      </c>
-      <c r="F77" t="s">
+      <c r="C77" s="10">
+        <v>43024</v>
+      </c>
+      <c r="D77" s="11">
+        <v>0.87430555555555556</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F77" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G77" t="s">
-        <v>21</v>
-      </c>
-      <c r="H77" t="s">
-        <v>58</v>
+      <c r="G77" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H77" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="I77" t="s">
         <v>55</v>
@@ -3333,64 +3330,64 @@
         <v>55</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B78" t="s">
         <v>37</v>
       </c>
       <c r="C78" s="1">
-        <v>42908</v>
+        <v>42855</v>
       </c>
       <c r="D78" s="2">
-        <v>0.93402777777777779</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E78" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F78" t="s">
         <v>67</v>
       </c>
       <c r="G78" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="H78" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I78" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="J78" t="s">
+        <v>22</v>
+      </c>
+      <c r="K78" t="s">
         <v>55</v>
       </c>
-      <c r="K78" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" s="9" t="s">
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" t="s">
         <v>47</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C79" s="10">
+      <c r="B79" t="s">
+        <v>43</v>
+      </c>
+      <c r="C79" s="1">
         <v>43024</v>
       </c>
-      <c r="D79" s="11">
+      <c r="D79" s="2">
         <v>0.87430555555555556</v>
       </c>
-      <c r="E79" s="9" t="s">
+      <c r="E79" t="s">
         <v>25</v>
       </c>
-      <c r="F79" s="9" t="s">
+      <c r="F79" t="s">
         <v>67</v>
       </c>
-      <c r="G79" s="9" t="s">
+      <c r="G79" t="s">
         <v>48</v>
       </c>
-      <c r="H79" s="9" t="s">
+      <c r="H79" t="s">
         <v>63</v>
       </c>
       <c r="I79" t="s">
@@ -3403,179 +3400,144 @@
         <v>55</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>50</v>
-      </c>
-      <c r="B80" t="s">
-        <v>37</v>
-      </c>
-      <c r="C80" s="1">
-        <v>42855</v>
-      </c>
-      <c r="D80" s="2">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E80" t="s">
-        <v>11</v>
-      </c>
-      <c r="F80" t="s">
+    <row r="80" spans="1:11">
+      <c r="A80" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D80" s="5">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G80" t="s">
+      <c r="G80" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H80" t="s">
+      <c r="H80" s="3" t="s">
         <v>58</v>
       </c>
       <c r="I80" t="s">
         <v>55</v>
       </c>
-      <c r="J80" t="s">
-        <v>22</v>
+      <c r="J80" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="K80" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11">
       <c r="A81" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B81" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C81" s="1">
-        <v>43024</v>
+        <v>42829</v>
       </c>
       <c r="D81" s="2">
-        <v>0.87430555555555556</v>
+        <v>0.89930555555555547</v>
       </c>
       <c r="E81" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F81" t="s">
         <v>67</v>
       </c>
       <c r="G81" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H81" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I81" t="s">
         <v>55</v>
       </c>
       <c r="J81" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="K81" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B82" s="3" t="s">
+    <row r="82" spans="1:11">
+      <c r="A82" t="s">
+        <v>72</v>
+      </c>
+      <c r="B82" t="s">
         <v>64</v>
       </c>
-      <c r="C82" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D82" s="5">
-        <v>8.8888888888888892E-2</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" s="3" t="s">
+      <c r="C82" s="1">
+        <v>42856</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E82" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" t="s">
         <v>67</v>
       </c>
-      <c r="G82" s="3" t="s">
+      <c r="G82" t="s">
         <v>21</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="H82" t="s">
         <v>58</v>
       </c>
       <c r="I82" t="s">
         <v>55</v>
       </c>
-      <c r="J82" s="3" t="s">
-        <v>44</v>
+      <c r="J82" t="s">
+        <v>62</v>
       </c>
       <c r="K82" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B83" t="s">
-        <v>64</v>
-      </c>
-      <c r="C83" s="1">
-        <v>42829</v>
-      </c>
-      <c r="D83" s="2">
-        <v>0.89930555555555547</v>
-      </c>
-      <c r="E83" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83" t="s">
-        <v>67</v>
-      </c>
-      <c r="G83" t="s">
-        <v>14</v>
-      </c>
-      <c r="H83" t="s">
-        <v>57</v>
-      </c>
-      <c r="I83" t="s">
-        <v>55</v>
-      </c>
-      <c r="J83" t="s">
-        <v>22</v>
-      </c>
-      <c r="K83" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11">
       <c r="A84" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="B84" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C84" s="1">
-        <v>42856</v>
+        <v>42908</v>
       </c>
       <c r="D84" s="2">
-        <v>1.3888888888888888E-2</v>
+        <v>0.93402777777777779</v>
       </c>
       <c r="E84" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F84" t="s">
         <v>67</v>
       </c>
       <c r="G84" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="H84" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I84" t="s">
+        <v>44</v>
+      </c>
+      <c r="J84" t="s">
         <v>55</v>
       </c>
-      <c r="J84" t="s">
-        <v>62</v>
-      </c>
       <c r="K84" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>